<commit_message>
Commit prior to cleanup for publication
</commit_message>
<xml_diff>
--- a/Classification_of_pandemic_cases.xlsx
+++ b/Classification_of_pandemic_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieg/Dropbox/R/2018_seasonal_flu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F674A-1410-8146-9A5C-4C13B08D182E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2A8846-7037-2F4E-BB89-AC201585C466}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{044AC8B0-38AC-8C4E-B18A-6638521280DB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Jan</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Arizona Data</t>
   </si>
   <si>
-    <t>ref: https://azdhs.gov/documents/preparedness/epidemiology-disease-control/flu/surveillance/2009-2010-influenza-summary-h1n1.pdf</t>
-  </si>
-  <si>
     <t>These AZ cases considered part of the 2009 pandemic.</t>
   </si>
   <si>
@@ -128,52 +125,21 @@
     <t>Starts 1990s, but only the "season" defined from week 40-week 39, is reported. No other date info given.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">These cases </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not considered part of the pandemic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, because I have no way to separate seasonal H1N1 cases early in the season from pandemic cases late in the season. I think most H1N1 cases reported in this time period represent early, seasonaly circulation, NOT pandemic circulation.  AZDHS reports that they had limited capacity to subtype pandemic H1N1 cases until Oct. 2009, and so few pandemic cases from this time period  were tested to subtype.</t>
-    </r>
-  </si>
-  <si>
     <t>cases repoted during 08-09 season</t>
   </si>
   <si>
     <t>cases reported during 09-10 season</t>
+  </si>
+  <si>
+    <t>These cases have a distinct age distribution and there are many more of them than recorded in pre-2009 seasonal circulation. Although some pre-pandemic seasonal cases may included, we'll consider these part of the 2009 pandemic.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -419,58 +385,16 @@
   </cellStyleXfs>
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -479,6 +403,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,11 +452,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,44 +464,57 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,7 +839,7 @@
   <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="B13" sqref="B13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -883,538 +849,535 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="B2" s="2">
+      <c r="B2" s="44">
         <v>2008</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43">
         <v>2009</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="2">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44">
         <v>2010</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AA3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="44">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="45" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="46"/>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="3"/>
-    </row>
-    <row r="5" spans="1:29" s="3" customFormat="1" ht="34">
-      <c r="A5" s="40" t="s">
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="39"/>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" s="1" customFormat="1" ht="34">
+      <c r="A5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="23" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:29" ht="39" customHeight="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="12" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="11" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="14" t="s">
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="10"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:29" ht="6" customHeight="1">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="24"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
     </row>
     <row r="8" spans="1:29" ht="34">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="22" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" spans="1:29" ht="34">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="6"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="33"/>
+    </row>
+    <row r="11" spans="1:29" ht="6" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+    </row>
+    <row r="12" spans="1:29" ht="16" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="26"/>
+    </row>
+    <row r="13" spans="1:29" ht="76" customHeight="1">
+      <c r="A13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="20"/>
-    </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="17"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="36"/>
-    </row>
-    <row r="11" spans="1:29" ht="6" customHeight="1">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
-    </row>
-    <row r="12" spans="1:29" ht="16" customHeight="1">
-      <c r="A12" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="25" t="s">
+      <c r="B13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="27"/>
-    </row>
-    <row r="13" spans="1:29" ht="76" customHeight="1">
-      <c r="A13" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="31"/>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
     </row>
     <row r="14" spans="1:29">
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="21"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
     </row>
     <row r="19" spans="11:13">
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="11:13">
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="11:13">
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" spans="11:13">
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="11:13">
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="11:13">
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="11:13">
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" spans="11:13">
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" spans="11:13">
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="N14:Y14"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="N12:Y12"/>
-    <mergeCell ref="Z12:AB12"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="N13:Y13"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="Q2:AB2"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="B4:G4"/>
     <mergeCell ref="N10:Y10"/>
     <mergeCell ref="Z13:AB13"/>
     <mergeCell ref="A5:A6"/>
@@ -1423,12 +1386,12 @@
     <mergeCell ref="N9:S9"/>
     <mergeCell ref="T9:Y9"/>
     <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="Q2:AB2"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="N14:Y14"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="N12:Y12"/>
+    <mergeCell ref="Z12:AB12"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="N13:Y13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>